<commit_message>
feat : update new version V 1.0.1
</commit_message>
<xml_diff>
--- a/public/DataUser/data-siswa-sma-megatama[untuk-pp].xlsx
+++ b/public/DataUser/data-siswa-sma-megatama[untuk-pp].xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIN 10\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEA66AF-127C-45F7-BC29-3DAE7C421323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24954D4-354A-4C73-8040-880D5C9BD1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{764C0629-A8AF-41BF-9117-334BE5AB9392}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{764C0629-A8AF-41BF-9117-334BE5AB9392}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_Sheet1" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="92">
   <si>
     <t>nama</t>
   </si>
@@ -312,14 +312,20 @@
     <t>SITI NURHALIMAH</t>
   </si>
   <si>
-    <t>IPS</t>
+    <t>Teknik Sepeda Motor</t>
+  </si>
+  <si>
+    <t>Teknik Kendaraan Ringan</t>
+  </si>
+  <si>
+    <t>Teknik Listrik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +337,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -369,15 +381,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{8DE3B54F-A311-4EBA-B457-19207156D250}"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -392,16 +417,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,15 +453,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEF5842F-A883-4D15-A90F-7B9A6FA42762}" name="Table_Table_Sheet1" displayName="Table_Table_Sheet1" ref="A1:I78" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I78" xr:uid="{DEF5842F-A883-4D15-A90F-7B9A6FA42762}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A2D9B9E0-533A-479E-9B99-4E6393DEBD7A}" uniqueName="1" name="nama" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{A2D9B9E0-533A-479E-9B99-4E6393DEBD7A}" uniqueName="1" name="nama" queryTableFieldId="1" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{929EA0C4-BFAE-4247-A32C-6832A3FC999C}" uniqueName="2" name="nisn" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{AD868D46-2D18-4434-B5F5-278AD17DAEE0}" uniqueName="3" name="jenis_kelamin" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{AD868D46-2D18-4434-B5F5-278AD17DAEE0}" uniqueName="3" name="jenis_kelamin" queryTableFieldId="3" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{671671BC-60D9-4F37-88E3-C3F1F0C70D2A}" uniqueName="4" name="wali_id" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{B9448828-CAE0-4739-8F4F-F1C0574BE8A1}" uniqueName="5" name="wali_status" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{480FFB32-6AFC-4170-BC01-7C568D5AC880}" uniqueName="6" name="jurusan" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B9448828-CAE0-4739-8F4F-F1C0574BE8A1}" uniqueName="5" name="wali_status" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{480FFB32-6AFC-4170-BC01-7C568D5AC880}" uniqueName="6" name="jurusan" queryTableFieldId="6" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{464FDE8F-41C8-4899-B0B4-DB1A52F217CD}" uniqueName="7" name="kelas" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{8F6D1168-0F6F-4C24-B89A-E16EFA772E54}" uniqueName="8" name="angkatan" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{D708CF7A-1589-43D4-B92B-EA22AABFD8C8}" uniqueName="9" name="biaya_id" queryTableFieldId="9" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{D708CF7A-1589-43D4-B92B-EA22AABFD8C8}" uniqueName="9" name="biaya_id" queryTableFieldId="9" dataDxfId="1">
       <calculatedColumnFormula>Table_Table_Sheet1[[#This Row],[angkatan]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -753,23 +768,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7081F7-E123-4F07-A949-2BE17D2132F9}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F51"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:F78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -798,7 +813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -814,7 +829,7 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G2">
@@ -827,7 +842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -843,7 +858,7 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G3">
@@ -856,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -872,7 +887,7 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G4">
@@ -885,7 +900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -901,7 +916,7 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G5">
@@ -914,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -930,7 +945,7 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G6">
@@ -943,7 +958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -959,8 +974,8 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" t="s">
-        <v>89</v>
+      <c r="F7" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G7">
         <v>10</v>
@@ -972,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -988,8 +1003,8 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
-        <v>89</v>
+      <c r="F8" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G8">
         <v>10</v>
@@ -1001,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1017,8 +1032,8 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
-        <v>89</v>
+      <c r="F9" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G9">
         <v>10</v>
@@ -1030,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1046,8 +1061,8 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="F10" t="s">
-        <v>89</v>
+      <c r="F10" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G10">
         <v>10</v>
@@ -1059,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1075,8 +1090,8 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
-        <v>89</v>
+      <c r="F11" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -1088,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1104,8 +1119,8 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" t="s">
-        <v>89</v>
+      <c r="F12" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G12">
         <v>10</v>
@@ -1117,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1133,8 +1148,8 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="F13" t="s">
-        <v>89</v>
+      <c r="F13" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G13">
         <v>10</v>
@@ -1146,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1162,8 +1177,8 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
-      <c r="F14" t="s">
-        <v>89</v>
+      <c r="F14" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G14">
         <v>10</v>
@@ -1175,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1191,8 +1206,8 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="F15" t="s">
-        <v>89</v>
+      <c r="F15" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G15">
         <v>10</v>
@@ -1204,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -1220,8 +1235,8 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="F16" t="s">
-        <v>89</v>
+      <c r="F16" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G16">
         <v>10</v>
@@ -1233,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1249,8 +1264,8 @@
       <c r="E17" t="s">
         <v>9</v>
       </c>
-      <c r="F17" t="s">
-        <v>89</v>
+      <c r="F17" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G17">
         <v>10</v>
@@ -1262,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1278,8 +1293,8 @@
       <c r="E18" t="s">
         <v>9</v>
       </c>
-      <c r="F18" t="s">
-        <v>89</v>
+      <c r="F18" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G18">
         <v>10</v>
@@ -1291,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1307,8 +1322,8 @@
       <c r="E19" t="s">
         <v>9</v>
       </c>
-      <c r="F19" t="s">
-        <v>89</v>
+      <c r="F19" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G19">
         <v>10</v>
@@ -1320,7 +1335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1336,8 +1351,8 @@
       <c r="E20" t="s">
         <v>9</v>
       </c>
-      <c r="F20" t="s">
-        <v>89</v>
+      <c r="F20" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G20">
         <v>10</v>
@@ -1349,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -1365,8 +1380,8 @@
       <c r="E21" t="s">
         <v>9</v>
       </c>
-      <c r="F21" t="s">
-        <v>89</v>
+      <c r="F21" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G21">
         <v>10</v>
@@ -1378,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1394,8 +1409,8 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
-      <c r="F22" t="s">
-        <v>89</v>
+      <c r="F22" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G22">
         <v>11</v>
@@ -1407,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1423,8 +1438,8 @@
       <c r="E23" t="s">
         <v>9</v>
       </c>
-      <c r="F23" t="s">
-        <v>89</v>
+      <c r="F23" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G23">
         <v>11</v>
@@ -1436,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1452,8 +1467,8 @@
       <c r="E24" t="s">
         <v>9</v>
       </c>
-      <c r="F24" t="s">
-        <v>89</v>
+      <c r="F24" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G24">
         <v>11</v>
@@ -1465,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1481,8 +1496,8 @@
       <c r="E25" t="s">
         <v>9</v>
       </c>
-      <c r="F25" t="s">
-        <v>89</v>
+      <c r="F25" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G25">
         <v>11</v>
@@ -1494,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1510,8 +1525,8 @@
       <c r="E26" t="s">
         <v>9</v>
       </c>
-      <c r="F26" t="s">
-        <v>89</v>
+      <c r="F26" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G26">
         <v>11</v>
@@ -1523,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1539,8 +1554,8 @@
       <c r="E27" t="s">
         <v>9</v>
       </c>
-      <c r="F27" t="s">
-        <v>89</v>
+      <c r="F27" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G27">
         <v>11</v>
@@ -1552,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1568,8 +1583,8 @@
       <c r="E28" t="s">
         <v>9</v>
       </c>
-      <c r="F28" t="s">
-        <v>89</v>
+      <c r="F28" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G28">
         <v>11</v>
@@ -1581,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1597,8 +1612,8 @@
       <c r="E29" t="s">
         <v>9</v>
       </c>
-      <c r="F29" t="s">
-        <v>89</v>
+      <c r="F29" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G29">
         <v>11</v>
@@ -1610,7 +1625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1626,8 +1641,8 @@
       <c r="E30" t="s">
         <v>9</v>
       </c>
-      <c r="F30" t="s">
-        <v>89</v>
+      <c r="F30" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G30">
         <v>11</v>
@@ -1639,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -1655,8 +1670,8 @@
       <c r="E31" t="s">
         <v>9</v>
       </c>
-      <c r="F31" t="s">
-        <v>89</v>
+      <c r="F31" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G31">
         <v>11</v>
@@ -1668,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1684,8 +1699,8 @@
       <c r="E32" t="s">
         <v>9</v>
       </c>
-      <c r="F32" t="s">
-        <v>89</v>
+      <c r="F32" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G32">
         <v>11</v>
@@ -1697,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
@@ -1713,8 +1728,8 @@
       <c r="E33" t="s">
         <v>9</v>
       </c>
-      <c r="F33" t="s">
-        <v>89</v>
+      <c r="F33" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G33">
         <v>11</v>
@@ -1726,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
@@ -1742,8 +1757,8 @@
       <c r="E34" t="s">
         <v>9</v>
       </c>
-      <c r="F34" t="s">
-        <v>89</v>
+      <c r="F34" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G34">
         <v>11</v>
@@ -1755,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
@@ -1771,8 +1786,8 @@
       <c r="E35" t="s">
         <v>9</v>
       </c>
-      <c r="F35" t="s">
-        <v>89</v>
+      <c r="F35" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G35">
         <v>11</v>
@@ -1784,7 +1799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -1800,8 +1815,8 @@
       <c r="E36" t="s">
         <v>9</v>
       </c>
-      <c r="F36" t="s">
-        <v>89</v>
+      <c r="F36" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G36">
         <v>11</v>
@@ -1813,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>47</v>
       </c>
@@ -1829,8 +1844,8 @@
       <c r="E37" t="s">
         <v>9</v>
       </c>
-      <c r="F37" t="s">
-        <v>89</v>
+      <c r="F37" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G37">
         <v>11</v>
@@ -1842,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -1858,8 +1873,8 @@
       <c r="E38" t="s">
         <v>9</v>
       </c>
-      <c r="F38" t="s">
-        <v>89</v>
+      <c r="F38" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G38">
         <v>11</v>
@@ -1871,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
@@ -1887,8 +1902,8 @@
       <c r="E39" t="s">
         <v>9</v>
       </c>
-      <c r="F39" t="s">
-        <v>89</v>
+      <c r="F39" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G39">
         <v>11</v>
@@ -1900,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
@@ -1916,8 +1931,8 @@
       <c r="E40" t="s">
         <v>9</v>
       </c>
-      <c r="F40" t="s">
-        <v>89</v>
+      <c r="F40" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G40">
         <v>11</v>
@@ -1929,7 +1944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
@@ -1945,8 +1960,8 @@
       <c r="E41" t="s">
         <v>9</v>
       </c>
-      <c r="F41" t="s">
-        <v>89</v>
+      <c r="F41" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G41">
         <v>11</v>
@@ -1958,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>52</v>
       </c>
@@ -1974,8 +1989,8 @@
       <c r="E42" t="s">
         <v>9</v>
       </c>
-      <c r="F42" t="s">
-        <v>89</v>
+      <c r="F42" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G42">
         <v>11</v>
@@ -1987,7 +2002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>53</v>
       </c>
@@ -2003,8 +2018,8 @@
       <c r="E43" t="s">
         <v>9</v>
       </c>
-      <c r="F43" t="s">
-        <v>89</v>
+      <c r="F43" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G43">
         <v>11</v>
@@ -2016,7 +2031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
@@ -2032,8 +2047,8 @@
       <c r="E44" t="s">
         <v>9</v>
       </c>
-      <c r="F44" t="s">
-        <v>89</v>
+      <c r="F44" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G44">
         <v>11</v>
@@ -2045,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>55</v>
       </c>
@@ -2061,8 +2076,8 @@
       <c r="E45" t="s">
         <v>9</v>
       </c>
-      <c r="F45" t="s">
-        <v>89</v>
+      <c r="F45" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G45">
         <v>11</v>
@@ -2074,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>56</v>
       </c>
@@ -2090,8 +2105,8 @@
       <c r="E46" t="s">
         <v>9</v>
       </c>
-      <c r="F46" t="s">
-        <v>89</v>
+      <c r="F46" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G46">
         <v>11</v>
@@ -2103,7 +2118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>57</v>
       </c>
@@ -2119,8 +2134,8 @@
       <c r="E47" t="s">
         <v>9</v>
       </c>
-      <c r="F47" t="s">
-        <v>89</v>
+      <c r="F47" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G47">
         <v>11</v>
@@ -2132,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>58</v>
       </c>
@@ -2148,8 +2163,8 @@
       <c r="E48" t="s">
         <v>9</v>
       </c>
-      <c r="F48" t="s">
-        <v>89</v>
+      <c r="F48" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G48">
         <v>11</v>
@@ -2161,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
@@ -2177,8 +2192,8 @@
       <c r="E49" t="s">
         <v>9</v>
       </c>
-      <c r="F49" t="s">
-        <v>89</v>
+      <c r="F49" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G49">
         <v>11</v>
@@ -2190,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>60</v>
       </c>
@@ -2206,8 +2221,8 @@
       <c r="E50" t="s">
         <v>9</v>
       </c>
-      <c r="F50" t="s">
-        <v>89</v>
+      <c r="F50" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G50">
         <v>11</v>
@@ -2219,7 +2234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>61</v>
       </c>
@@ -2235,8 +2250,8 @@
       <c r="E51" t="s">
         <v>9</v>
       </c>
-      <c r="F51" t="s">
-        <v>89</v>
+      <c r="F51" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G51">
         <v>11</v>
@@ -2248,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>62</v>
       </c>
@@ -2264,8 +2279,8 @@
       <c r="E52" t="s">
         <v>9</v>
       </c>
-      <c r="F52" t="s">
-        <v>89</v>
+      <c r="F52" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G52">
         <v>12</v>
@@ -2277,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
@@ -2293,8 +2308,8 @@
       <c r="E53" t="s">
         <v>9</v>
       </c>
-      <c r="F53" t="s">
-        <v>89</v>
+      <c r="F53" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G53">
         <v>12</v>
@@ -2306,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>64</v>
       </c>
@@ -2322,8 +2337,8 @@
       <c r="E54" t="s">
         <v>9</v>
       </c>
-      <c r="F54" t="s">
-        <v>89</v>
+      <c r="F54" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G54">
         <v>12</v>
@@ -2335,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
@@ -2351,8 +2366,8 @@
       <c r="E55" t="s">
         <v>9</v>
       </c>
-      <c r="F55" t="s">
-        <v>89</v>
+      <c r="F55" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G55">
         <v>12</v>
@@ -2364,7 +2379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
@@ -2380,8 +2395,8 @@
       <c r="E56" t="s">
         <v>9</v>
       </c>
-      <c r="F56" t="s">
-        <v>89</v>
+      <c r="F56" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G56">
         <v>12</v>
@@ -2393,7 +2408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>67</v>
       </c>
@@ -2409,8 +2424,8 @@
       <c r="E57" t="s">
         <v>9</v>
       </c>
-      <c r="F57" t="s">
-        <v>89</v>
+      <c r="F57" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G57">
         <v>12</v>
@@ -2422,7 +2437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>68</v>
       </c>
@@ -2438,8 +2453,8 @@
       <c r="E58" t="s">
         <v>9</v>
       </c>
-      <c r="F58" t="s">
-        <v>89</v>
+      <c r="F58" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G58">
         <v>12</v>
@@ -2451,7 +2466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>69</v>
       </c>
@@ -2467,8 +2482,8 @@
       <c r="E59" t="s">
         <v>9</v>
       </c>
-      <c r="F59" t="s">
-        <v>89</v>
+      <c r="F59" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G59">
         <v>12</v>
@@ -2480,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
@@ -2496,8 +2511,8 @@
       <c r="E60" t="s">
         <v>9</v>
       </c>
-      <c r="F60" t="s">
-        <v>89</v>
+      <c r="F60" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G60">
         <v>12</v>
@@ -2509,7 +2524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>71</v>
       </c>
@@ -2525,8 +2540,8 @@
       <c r="E61" t="s">
         <v>9</v>
       </c>
-      <c r="F61" t="s">
-        <v>89</v>
+      <c r="F61" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G61">
         <v>12</v>
@@ -2538,7 +2553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>72</v>
       </c>
@@ -2554,8 +2569,8 @@
       <c r="E62" t="s">
         <v>9</v>
       </c>
-      <c r="F62" t="s">
-        <v>89</v>
+      <c r="F62" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G62">
         <v>12</v>
@@ -2567,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>
@@ -2583,8 +2598,8 @@
       <c r="E63" t="s">
         <v>9</v>
       </c>
-      <c r="F63" t="s">
-        <v>89</v>
+      <c r="F63" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G63">
         <v>12</v>
@@ -2596,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>74</v>
       </c>
@@ -2612,8 +2627,8 @@
       <c r="E64" t="s">
         <v>9</v>
       </c>
-      <c r="F64" t="s">
-        <v>89</v>
+      <c r="F64" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G64">
         <v>12</v>
@@ -2625,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>75</v>
       </c>
@@ -2641,8 +2656,8 @@
       <c r="E65" t="s">
         <v>9</v>
       </c>
-      <c r="F65" t="s">
-        <v>89</v>
+      <c r="F65" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G65">
         <v>12</v>
@@ -2654,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>76</v>
       </c>
@@ -2670,8 +2685,8 @@
       <c r="E66" t="s">
         <v>9</v>
       </c>
-      <c r="F66" t="s">
-        <v>89</v>
+      <c r="F66" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G66">
         <v>12</v>
@@ -2683,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>77</v>
       </c>
@@ -2699,8 +2714,8 @@
       <c r="E67" t="s">
         <v>9</v>
       </c>
-      <c r="F67" t="s">
-        <v>89</v>
+      <c r="F67" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G67">
         <v>12</v>
@@ -2712,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>78</v>
       </c>
@@ -2728,8 +2743,8 @@
       <c r="E68" t="s">
         <v>9</v>
       </c>
-      <c r="F68" t="s">
-        <v>89</v>
+      <c r="F68" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G68">
         <v>12</v>
@@ -2741,7 +2756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>79</v>
       </c>
@@ -2757,8 +2772,8 @@
       <c r="E69" t="s">
         <v>9</v>
       </c>
-      <c r="F69" t="s">
-        <v>89</v>
+      <c r="F69" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G69">
         <v>12</v>
@@ -2770,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>80</v>
       </c>
@@ -2786,8 +2801,8 @@
       <c r="E70" t="s">
         <v>9</v>
       </c>
-      <c r="F70" t="s">
-        <v>89</v>
+      <c r="F70" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G70">
         <v>12</v>
@@ -2799,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>81</v>
       </c>
@@ -2815,8 +2830,8 @@
       <c r="E71" t="s">
         <v>9</v>
       </c>
-      <c r="F71" t="s">
-        <v>89</v>
+      <c r="F71" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G71">
         <v>12</v>
@@ -2828,7 +2843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>82</v>
       </c>
@@ -2844,8 +2859,8 @@
       <c r="E72" t="s">
         <v>9</v>
       </c>
-      <c r="F72" t="s">
-        <v>89</v>
+      <c r="F72" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G72">
         <v>12</v>
@@ -2857,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>83</v>
       </c>
@@ -2873,8 +2888,8 @@
       <c r="E73" t="s">
         <v>9</v>
       </c>
-      <c r="F73" t="s">
-        <v>89</v>
+      <c r="F73" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G73">
         <v>12</v>
@@ -2886,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
@@ -2902,8 +2917,8 @@
       <c r="E74" t="s">
         <v>9</v>
       </c>
-      <c r="F74" t="s">
-        <v>89</v>
+      <c r="F74" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G74">
         <v>12</v>
@@ -2915,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>85</v>
       </c>
@@ -2931,8 +2946,8 @@
       <c r="E75" t="s">
         <v>9</v>
       </c>
-      <c r="F75" t="s">
-        <v>89</v>
+      <c r="F75" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G75">
         <v>12</v>
@@ -2944,7 +2959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>86</v>
       </c>
@@ -2960,8 +2975,8 @@
       <c r="E76" t="s">
         <v>9</v>
       </c>
-      <c r="F76" t="s">
-        <v>89</v>
+      <c r="F76" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G76">
         <v>12</v>
@@ -2973,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>87</v>
       </c>
@@ -2989,8 +3004,8 @@
       <c r="E77" t="s">
         <v>9</v>
       </c>
-      <c r="F77" t="s">
-        <v>89</v>
+      <c r="F77" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G77">
         <v>12</v>
@@ -3002,7 +3017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>88</v>
       </c>
@@ -3018,8 +3033,8 @@
       <c r="E78" t="s">
         <v>9</v>
       </c>
-      <c r="F78" t="s">
-        <v>89</v>
+      <c r="F78" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G78">
         <v>12</v>
@@ -3032,8 +3047,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:H78">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  <conditionalFormatting sqref="A1:H1 A2:E78 G2:H78">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3048,7 +3063,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>